<commit_message>
Organize tabs in dev-roadmap
</commit_message>
<xml_diff>
--- a/sis/dcraig327/research/dev-roadmap-checklist.xlsx
+++ b/sis/dcraig327/research/dev-roadmap-checklist.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Backend" sheetId="1" r:id="rId1"/>
-    <sheet name="Devops" sheetId="2" r:id="rId2"/>
-    <sheet name="Frontend" sheetId="3" r:id="rId3"/>
+    <sheet name="Frontend" sheetId="3" r:id="rId2"/>
+    <sheet name="Devops" sheetId="2" r:id="rId3"/>
     <sheet name="Projects" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -439,6 +439,9 @@
     <t>Never Stop Learning</t>
   </si>
   <si>
+    <t>Web Assembly vs JavaScript</t>
+  </si>
+  <si>
     <t>load balancing</t>
   </si>
   <si>
@@ -509,9 +512,6 @@
   </si>
   <si>
     <t>to automate</t>
-  </si>
-  <si>
-    <t>Web Assembly vs JavaScript</t>
   </si>
   <si>
     <t>Projects</t>
@@ -561,9 +561,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -598,7 +598,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -608,22 +608,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -652,6 +636,29 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -667,39 +674,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -725,6 +702,29 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -753,43 +753,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,121 +909,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,7 +933,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -953,15 +953,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -973,6 +964,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -994,6 +1000,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1002,162 +1026,138 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2180,6 +2180,28 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2190,121 +2212,99 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>